<commit_message>
Added in the theoretical forrays from the beginning of the semester. Now finally going into the newly discovered wins.
</commit_message>
<xml_diff>
--- a/Excell Analysis/Dec-7-V9.xlsx
+++ b/Excell Analysis/Dec-7-V9.xlsx
@@ -606,6 +606,212 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$58:$I$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$58:$K$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -762,6 +968,7 @@
     <sheetView tabSelected="1" zoomScale="169" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
 </chartsheet>
 </file>
@@ -1117,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="R83" sqref="R83"/>
+    <sheetView topLeftCell="B81" workbookViewId="0">
+      <selection activeCell="K124" sqref="K124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1177,8 +1384,8 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <f>CEILING(J2/H2,1)</f>
-        <v>1</v>
+        <f>CEILING(J2/H2,1)*H2</f>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1218,8 +1425,8 @@
         <v>1</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K66" si="8">CEILING(J3/H3,1)</f>
-        <v>1</v>
+        <f t="shared" ref="K3:K66" si="8">CEILING(J3/H3,1)*H3</f>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1260,7 +1467,7 @@
       </c>
       <c r="K4">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1301,7 +1508,7 @@
       </c>
       <c r="K5">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1342,7 +1549,7 @@
       </c>
       <c r="K6">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1383,7 +1590,7 @@
       </c>
       <c r="K7">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1424,7 +1631,7 @@
       </c>
       <c r="K8">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1465,7 +1672,7 @@
       </c>
       <c r="K9">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1506,7 +1713,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1547,7 +1754,7 @@
       </c>
       <c r="K11">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1588,7 +1795,7 @@
       </c>
       <c r="K12">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1629,7 +1836,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1670,7 +1877,7 @@
       </c>
       <c r="K14">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1711,7 +1918,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1752,7 +1959,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1793,7 +2000,7 @@
       </c>
       <c r="K17">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1834,7 +2041,7 @@
       </c>
       <c r="K18">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1875,7 +2082,7 @@
       </c>
       <c r="K19">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1916,7 +2123,7 @@
       </c>
       <c r="K20">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1957,7 +2164,7 @@
       </c>
       <c r="K21">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1998,7 +2205,7 @@
       </c>
       <c r="K22">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -2039,7 +2246,7 @@
       </c>
       <c r="K23">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -2080,7 +2287,7 @@
       </c>
       <c r="K24">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -2121,7 +2328,7 @@
       </c>
       <c r="K25">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -2162,7 +2369,7 @@
       </c>
       <c r="K26">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -2203,7 +2410,7 @@
       </c>
       <c r="K27">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -2244,7 +2451,7 @@
       </c>
       <c r="K28">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -2285,7 +2492,7 @@
       </c>
       <c r="K29">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -2326,7 +2533,7 @@
       </c>
       <c r="K30">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -2367,7 +2574,7 @@
       </c>
       <c r="K31">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -2408,7 +2615,7 @@
       </c>
       <c r="K32">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -2449,7 +2656,7 @@
       </c>
       <c r="K33">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -2490,7 +2697,7 @@
       </c>
       <c r="K34">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -2531,7 +2738,7 @@
       </c>
       <c r="K35">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -2572,7 +2779,7 @@
       </c>
       <c r="K36">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -2613,7 +2820,7 @@
       </c>
       <c r="K37">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -2654,7 +2861,7 @@
       </c>
       <c r="K38">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -2695,7 +2902,7 @@
       </c>
       <c r="K39">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -2736,7 +2943,7 @@
       </c>
       <c r="K40">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -2777,7 +2984,7 @@
       </c>
       <c r="K41">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -2818,7 +3025,7 @@
       </c>
       <c r="K42">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -2859,7 +3066,7 @@
       </c>
       <c r="K43">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -2900,7 +3107,7 @@
       </c>
       <c r="K44">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -2941,7 +3148,7 @@
       </c>
       <c r="K45">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2982,7 +3189,7 @@
       </c>
       <c r="K46">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -3023,7 +3230,7 @@
       </c>
       <c r="K47">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -3064,7 +3271,7 @@
       </c>
       <c r="K48">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -3105,7 +3312,7 @@
       </c>
       <c r="K49">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -3146,7 +3353,7 @@
       </c>
       <c r="K50">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -3187,7 +3394,7 @@
       </c>
       <c r="K51">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -3228,7 +3435,7 @@
       </c>
       <c r="K52">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -3269,7 +3476,7 @@
       </c>
       <c r="K53">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -3310,7 +3517,7 @@
       </c>
       <c r="K54">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -3351,7 +3558,7 @@
       </c>
       <c r="K55">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -3392,7 +3599,7 @@
       </c>
       <c r="K56">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -3433,7 +3640,7 @@
       </c>
       <c r="K57">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -3474,7 +3681,7 @@
       </c>
       <c r="K58">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -3515,7 +3722,7 @@
       </c>
       <c r="K59">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -3556,7 +3763,7 @@
       </c>
       <c r="K60">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -3597,7 +3804,7 @@
       </c>
       <c r="K61">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -3638,7 +3845,7 @@
       </c>
       <c r="K62">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="63" spans="1:11">
@@ -3679,7 +3886,7 @@
       </c>
       <c r="K63">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -3720,7 +3927,7 @@
       </c>
       <c r="K64">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:11">
@@ -3761,7 +3968,7 @@
       </c>
       <c r="K65">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="66" spans="1:11">
@@ -3802,7 +4009,7 @@
       </c>
       <c r="K66">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="67" spans="1:11">
@@ -3842,8 +4049,8 @@
         <v>23</v>
       </c>
       <c r="K67">
-        <f t="shared" ref="K67:K121" si="17">CEILING(J67/H67,1)</f>
-        <v>3</v>
+        <f t="shared" ref="K67:K121" si="17">CEILING(J67/H67,1)*H67</f>
+        <v>24</v>
       </c>
     </row>
     <row r="68" spans="1:11">
@@ -3884,7 +4091,7 @@
       </c>
       <c r="K68">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -3925,7 +4132,7 @@
       </c>
       <c r="K69">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -3966,7 +4173,7 @@
       </c>
       <c r="K70">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -4007,7 +4214,7 @@
       </c>
       <c r="K71">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -4048,7 +4255,7 @@
       </c>
       <c r="K72">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -4089,7 +4296,7 @@
       </c>
       <c r="K73">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -4130,7 +4337,7 @@
       </c>
       <c r="K74">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -4171,7 +4378,7 @@
       </c>
       <c r="K75">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="76" spans="1:11">
@@ -4212,7 +4419,7 @@
       </c>
       <c r="K76">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="77" spans="1:11">
@@ -4253,7 +4460,7 @@
       </c>
       <c r="K77">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="78" spans="1:11">
@@ -4294,7 +4501,7 @@
       </c>
       <c r="K78">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="79" spans="1:11">
@@ -4335,7 +4542,7 @@
       </c>
       <c r="K79">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:11">
@@ -4376,7 +4583,7 @@
       </c>
       <c r="K80">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="81" spans="1:11">
@@ -4417,7 +4624,7 @@
       </c>
       <c r="K81">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="82" spans="1:11">
@@ -4458,7 +4665,7 @@
       </c>
       <c r="K82">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:11">
@@ -4499,7 +4706,7 @@
       </c>
       <c r="K83">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:11">
@@ -4540,7 +4747,7 @@
       </c>
       <c r="K84">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:11">
@@ -4581,7 +4788,7 @@
       </c>
       <c r="K85">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:11">
@@ -4622,7 +4829,7 @@
       </c>
       <c r="K86">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:11">
@@ -4663,7 +4870,7 @@
       </c>
       <c r="K87">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:11">
@@ -4704,7 +4911,7 @@
       </c>
       <c r="K88">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:11">
@@ -4745,7 +4952,7 @@
       </c>
       <c r="K89">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -4786,7 +4993,7 @@
       </c>
       <c r="K90">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="91" spans="1:11">
@@ -4827,7 +5034,7 @@
       </c>
       <c r="K91">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="92" spans="1:11">
@@ -4868,7 +5075,7 @@
       </c>
       <c r="K92">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="93" spans="1:11">
@@ -4909,7 +5116,7 @@
       </c>
       <c r="K93">
         <f t="shared" si="17"/>
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="94" spans="1:11">
@@ -4950,7 +5157,7 @@
       </c>
       <c r="K94">
         <f t="shared" si="17"/>
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="95" spans="1:11">
@@ -4991,7 +5198,7 @@
       </c>
       <c r="K95">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="96" spans="1:11">
@@ -5032,7 +5239,7 @@
       </c>
       <c r="K96">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="97" spans="1:11">
@@ -5073,7 +5280,7 @@
       </c>
       <c r="K97">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="98" spans="1:11">
@@ -5114,7 +5321,7 @@
       </c>
       <c r="K98">
         <f t="shared" si="17"/>
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="99" spans="1:11">
@@ -5155,7 +5362,7 @@
       </c>
       <c r="K99">
         <f t="shared" si="17"/>
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="100" spans="1:11">
@@ -5196,7 +5403,7 @@
       </c>
       <c r="K100">
         <f t="shared" si="17"/>
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="101" spans="1:11">
@@ -5237,7 +5444,7 @@
       </c>
       <c r="K101">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="102" spans="1:11">
@@ -5278,7 +5485,7 @@
       </c>
       <c r="K102">
         <f t="shared" si="17"/>
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="103" spans="1:11">
@@ -5319,7 +5526,7 @@
       </c>
       <c r="K103">
         <f t="shared" si="17"/>
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="104" spans="1:11">
@@ -5360,7 +5567,7 @@
       </c>
       <c r="K104">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="105" spans="1:11">
@@ -5401,7 +5608,7 @@
       </c>
       <c r="K105">
         <f t="shared" si="17"/>
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="106" spans="1:11">
@@ -5442,7 +5649,7 @@
       </c>
       <c r="K106">
         <f t="shared" si="17"/>
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="107" spans="1:11">
@@ -5483,7 +5690,7 @@
       </c>
       <c r="K107">
         <f t="shared" si="17"/>
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="108" spans="1:11">
@@ -5524,7 +5731,7 @@
       </c>
       <c r="K108">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="109" spans="1:11">
@@ -5565,7 +5772,7 @@
       </c>
       <c r="K109">
         <f t="shared" si="17"/>
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="110" spans="1:11">
@@ -5606,7 +5813,7 @@
       </c>
       <c r="K110">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="111" spans="1:11">
@@ -5647,7 +5854,7 @@
       </c>
       <c r="K111">
         <f t="shared" si="17"/>
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="112" spans="1:11">
@@ -5688,7 +5895,7 @@
       </c>
       <c r="K112">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="113" spans="1:11">
@@ -5729,7 +5936,7 @@
       </c>
       <c r="K113">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="114" spans="1:11">
@@ -5770,7 +5977,7 @@
       </c>
       <c r="K114">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="115" spans="1:11">
@@ -5811,7 +6018,7 @@
       </c>
       <c r="K115">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="116" spans="1:11">
@@ -5852,7 +6059,7 @@
       </c>
       <c r="K116">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="117" spans="1:11">
@@ -5893,7 +6100,7 @@
       </c>
       <c r="K117">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="118" spans="1:11">
@@ -5934,7 +6141,7 @@
       </c>
       <c r="K118">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="119" spans="1:11">
@@ -5975,7 +6182,7 @@
       </c>
       <c r="K119">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="120" spans="1:11">
@@ -6016,7 +6223,7 @@
       </c>
       <c r="K120">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="121" spans="1:11">
@@ -6057,7 +6264,7 @@
       </c>
       <c r="K121">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>